<commit_message>
Add write_csv, fix_duplicates, trim
</commit_message>
<xml_diff>
--- a/test_translations.xlsx
+++ b/test_translations.xlsx
@@ -20,20 +20,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="135">
   <si>
     <t xml:space="preserve">key</t>
   </si>
   <si>
-    <t xml:space="preserve">exported</t>
+    <t xml:space="preserve">exportable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_comment</t>
   </si>
   <si>
     <t xml:space="preserve">comment</t>
   </si>
   <si>
-    <t xml:space="preserve">is_comment</t>
-  </si>
-  <si>
     <t xml:space="preserve">en</t>
   </si>
   <si>
@@ -91,13 +91,16 @@
     <t xml:space="preserve">comment.generated</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes</t>
+    <t xml:space="preserve">True</t>
   </si>
   <si>
     <t xml:space="preserve">Generated by mobile dev tools - Do not modify</t>
   </si>
   <si>
     <t xml:space="preserve">menu.welcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">Title on menu header</t>
@@ -153,7 +156,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>! </t>
+      <t>!</t>
     </r>
   </si>
   <si>
@@ -346,7 +349,7 @@
     <t xml:space="preserve">문의하기</t>
   </si>
   <si>
-    <t xml:space="preserve"> تواصل</t>
+    <t xml:space="preserve">تواصل</t>
   </si>
   <si>
     <t xml:space="preserve">İletişim</t>
@@ -473,8 +476,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -545,8 +549,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -580,9 +588,9 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.44897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.89285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.5714285714286"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.41326530612245"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.969387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5255102040816"/>
@@ -596,7 +604,7 @@
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.0510204081633"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.6938775510204"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.5714285714286"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.25"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.77551020408163"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.9336734693878"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.8061224489796"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.6122448979592"/>
@@ -676,542 +684,569 @@
       <c r="A2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="E3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="P3" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>45</v>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="I4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="V4" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>62</v>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="H5" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="P5" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="R5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="R5" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="S5" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="T5" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="U5" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="U5" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="V5" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>80</v>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>82</v>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>83</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G7" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="L7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N7" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="0" t="s">
+      <c r="O7" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="V7" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="T7" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="V7" s="0" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>97</v>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>98</v>
-      </c>
       <c r="J8" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="O8" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="N8" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="P8" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="S8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="S8" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="T8" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="U8" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="U8" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="V8" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="0" t="s">
         <v>114</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>115</v>
+      </c>
       <c r="E9" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q9" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N9" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q9" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="S9" s="1" t="s">
+      <c r="R9" s="2" t="s">
         <v>128</v>
       </c>
+      <c r="S9" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="T9" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="U9" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="U9" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="V9" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="V10" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N10" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="O10" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="P10" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q10" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="T10" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="V10" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q11" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="V11" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N11" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="O11" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="P11" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q11" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="T11" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="V11" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve tokens parsing, unittests, fix booleans
</commit_message>
<xml_diff>
--- a/test_translations.xlsx
+++ b/test_translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="134">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">menu.welcome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">Title on menu header</t>
@@ -701,206 +698,197 @@
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="L3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="O3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="R3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="S3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="T3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="H4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="K4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="O4" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="P4" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="Q4" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="R4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="U4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="U4" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="V4" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="I5" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="K5" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="L5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="O5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="P5" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="O5" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="P5" s="0" t="s">
+      <c r="Q5" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="R5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="T5" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="T5" s="0" t="s">
+      <c r="U5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="V5" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -909,344 +897,326 @@
         <v>23</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D7" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="H7" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N7" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="K7" s="0" t="s">
+      <c r="O7" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="V7" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="T7" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="V7" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D8" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="I8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J8" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="J8" s="0" t="s">
+      <c r="K8" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="L8" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="0" t="s">
+      <c r="O8" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="P8" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="O8" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="P8" s="0" t="s">
+      <c r="Q8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="Q8" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="T8" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="T8" s="0" t="s">
+      <c r="U8" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="V8" s="0" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="F9" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="I9" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="J9" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="K9" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="L9" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="N9" s="0" t="s">
+      <c r="O9" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="O9" s="0" t="s">
+      <c r="P9" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="P9" s="0" t="s">
+      <c r="Q9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="Q9" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="R9" s="2" t="s">
+      <c r="S9" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="T9" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="T9" s="0" t="s">
+      <c r="U9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="V9" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="V9" s="0" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D10" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="G10" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="H10" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="I10" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="J10" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="K10" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="L10" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="N10" s="0" t="s">
+      <c r="O10" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="O10" s="0" t="s">
+      <c r="P10" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="P10" s="0" t="s">
+      <c r="Q10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="Q10" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="R10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="T10" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="T10" s="0" t="s">
+      <c r="U10" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="V10" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="V10" s="0" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D11" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="H11" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="I11" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="J11" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="K11" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="L11" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="N11" s="0" t="s">
+      <c r="O11" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="O11" s="0" t="s">
+      <c r="P11" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="P11" s="0" t="s">
+      <c r="Q11" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="R11" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="Q11" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="R11" s="2" t="s">
+      <c r="S11" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="T11" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="T11" s="0" t="s">
+      <c r="U11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="V11" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="V11" s="0" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>